<commit_message>
Hotove frontend akceptacne testy
</commit_message>
<xml_diff>
--- a/AkceptacneTesty/Book1.xlsx
+++ b/AkceptacneTesty/Book1.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adyno\Google_Drive\School\6.Sem\MTAA\FrontEnd\AkceptacneTesty\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FBD75C-D7AC-4616-BDFC-55BC6574C958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Test 1: Nákup knihy bez registrácie</t>
   </si>
@@ -67,57 +76,76 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Výsledok:</t>
+    <t>Test 4: Vymazanie knihy</t>
+  </si>
+  <si>
+    <t>Používateľ je prihlásený ako administrátor. A má prístup na internet.</t>
+  </si>
+  <si>
+    <t>Aplikácia informuje administrátora že kniha bola vymazaná. No v skutočnosti sa nevymazala.</t>
+  </si>
+  <si>
+    <t>1. Užívateľ klikne na tlačidlo profilu 2. Užívateľ klikne na tlačidlo Edit Book                                                     3. Na screene editovacieho formuláru klikne na tlačidlo delete book                                                     4. Aplikácia ho informuje že kniha bola vymazaná</t>
+  </si>
+  <si>
+    <t>Test 5: Dobitie kreditu</t>
+  </si>
+  <si>
+    <t>Používateľ je prihlásený a má prístup na internet.</t>
+  </si>
+  <si>
+    <t>Používateľ si úspešné dobije peňažný kredit do svojho účtu.</t>
+  </si>
+  <si>
+    <t>1. Používateľ klikne na tlačidlo profilu                                                    2. Používateľ klikne na tlačidlo Deposit                                                   3. Do fieldu "Enter Card ID" vyplní číslo karty                                              4. Do fieldu "Enter Amount of money" vyplní sumu ktorú chce na účet umiestniť                                       5. Klikne na tlačidlo deposit a bude presmerovaný na svoj balance screen aby videl že sa mu kredit doplnil.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="4">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -127,58 +155,80 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -376,21 +426,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="6350" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="12700" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="19050" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -407,7 +457,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" rotWithShape="0" algn="ctr" dir="5400000" dist="19050">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -457,222 +507,231 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}"/>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:D100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:C33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.14"/>
-    <col customWidth="1" min="3" max="3" width="29.43"/>
-    <col customWidth="1" min="4" max="11" width="8.71"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" customWidth="1"/>
+    <col min="4" max="11" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="2" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" ht="48.0" customHeight="1">
-      <c r="B3" s="3" t="s">
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="2:3" ht="48" customHeight="1">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="45.0" customHeight="1">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:3" ht="45" customHeight="1">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="102.0" customHeight="1">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="2:3" ht="102" customHeight="1">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1"/>
-    <row r="8" ht="14.25" customHeight="1"/>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="B9" s="1" t="s">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="8" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="9" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="B10" s="3" t="s">
+      <c r="C9" s="7"/>
+    </row>
+    <row r="10" spans="2:3" ht="57" customHeight="1">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:3" ht="49.2" customHeight="1">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="2:3" ht="153.6" customHeight="1">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1"/>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="B15" s="1" t="s">
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="15" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="B16" s="3" t="s">
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="2:3" ht="46.2" customHeight="1">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="2:4" ht="20.399999999999999" customHeight="1">
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:4" ht="97.8" customHeight="1">
+      <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B19" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="B22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="B23" s="3" t="s">
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="21" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="22" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="2:4" ht="54.6" customHeight="1">
+      <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="B24" s="3" t="s">
+      <c r="C23" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="49.2" customHeight="1">
+      <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="B25" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="121.2" customHeight="1">
+      <c r="B25" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="B26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="B29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="B30" s="3" t="s">
+      <c r="C25" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="2:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="2:4" ht="14.25" customHeight="1">
+      <c r="B29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7"/>
+    </row>
+    <row r="30" spans="2:4" ht="35.4" customHeight="1">
+      <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="B31" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="34.799999999999997" customHeight="1">
+      <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="B32" s="3" t="s">
+      <c r="C31" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="195.6" customHeight="1">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="B33" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+      <c r="C32" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="14.25" customHeight="1">
+      <c r="B33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="2:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -727,20 +786,18 @@
     <row r="100" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B19:C19"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Toto bude este zabava
</commit_message>
<xml_diff>
--- a/AkceptacneTesty/Book1.xlsx
+++ b/AkceptacneTesty/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adyno\Google_Drive\School\6.Sem\MTAA\FrontEnd\AkceptacneTesty\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FBD75C-D7AC-4616-BDFC-55BC6574C958}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B35C877-8804-47DB-9560-97C0361799AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,18 +76,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Test 4: Vymazanie knihy</t>
-  </si>
-  <si>
     <t>Používateľ je prihlásený ako administrátor. A má prístup na internet.</t>
   </si>
   <si>
-    <t>Aplikácia informuje administrátora že kniha bola vymazaná. No v skutočnosti sa nevymazala.</t>
-  </si>
-  <si>
-    <t>1. Užívateľ klikne na tlačidlo profilu 2. Užívateľ klikne na tlačidlo Edit Book                                                     3. Na screene editovacieho formuláru klikne na tlačidlo delete book                                                     4. Aplikácia ho informuje že kniha bola vymazaná</t>
-  </si>
-  <si>
     <t>Test 5: Dobitie kreditu</t>
   </si>
   <si>
@@ -98,6 +89,15 @@
   </si>
   <si>
     <t>1. Používateľ klikne na tlačidlo profilu                                                    2. Používateľ klikne na tlačidlo Deposit                                                   3. Do fieldu "Enter Card ID" vyplní číslo karty                                              4. Do fieldu "Enter Amount of money" vyplní sumu ktorú chce na účet umiestniť                                       5. Klikne na tlačidlo deposit a bude presmerovaný na svoj balance screen aby videl že sa mu kredit doplnil.</t>
+  </si>
+  <si>
+    <t>Test 4: Pridanie knihy</t>
+  </si>
+  <si>
+    <t>Aplikácia neinformuje používateľa že v knihe chýba PDF.</t>
+  </si>
+  <si>
+    <t>1. Užívateľ klikne na tlačidlo profilu 2. Užívateľ klikne na tlačidlo Add Book                                                     3. Na screene prídávacieho formuláru vyplní všetky polia ale nevyberie PDF.                                     4. Klikne úspešne na tlačidlo Submit 5. Kniha si pridá bez PDF</t>
   </si>
 </sst>
 </file>
@@ -193,15 +193,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,7 +515,7 @@
   <dimension ref="B1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C33"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -528,10 +528,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="2:3" ht="48" customHeight="1">
       <c r="B3" s="1" t="s">
@@ -558,18 +558,18 @@
       </c>
     </row>
     <row r="6" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="8" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="9" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="2:3" ht="57" customHeight="1">
       <c r="B10" s="1" t="s">
@@ -596,17 +596,17 @@
       </c>
     </row>
     <row r="13" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="15" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="8"/>
     </row>
     <row r="16" spans="2:3" ht="46.2" customHeight="1">
       <c r="B16" s="1" t="s">
@@ -636,25 +636,25 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="14.25" customHeight="1">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="21" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="22" spans="2:4" ht="14.25" customHeight="1">
-      <c r="B22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7"/>
+      <c r="B22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="2:4" ht="54.6" customHeight="1">
       <c r="B23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="49.2" customHeight="1">
@@ -662,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="121.2" customHeight="1">
@@ -670,29 +670,29 @@
         <v>5</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="14.25" customHeight="1">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="28" spans="2:4" ht="14.25" customHeight="1"/>
     <row r="29" spans="2:4" ht="14.25" customHeight="1">
-      <c r="B29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="7"/>
+      <c r="B29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="2:4" ht="35.4" customHeight="1">
       <c r="B30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="34.799999999999997" customHeight="1">
@@ -700,22 +700,22 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="195.6" customHeight="1">
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>25</v>
+      <c r="C32" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="14.25" customHeight="1">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="7"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" spans="2:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="2:3" ht="14.25" customHeight="1"/>

</xml_diff>